<commit_message>
we do a little bit of trolling
</commit_message>
<xml_diff>
--- a/templates/table.xlsx
+++ b/templates/table.xlsx
@@ -22,7 +22,7 @@
     <t>Deliverables</t>
   </si>
   <si>
-    <t>Waternarks</t>
+    <t>Watermarks</t>
   </si>
   <si>
     <t>Upload Destination</t>
@@ -224,7 +224,7 @@
     <tableColumn name="Client Name" id="1"/>
     <tableColumn name="Project Name" id="2"/>
     <tableColumn name="Deliverables" id="3"/>
-    <tableColumn name="Waternarks" id="4"/>
+    <tableColumn name="Watermarks" id="4"/>
     <tableColumn name="Upload Destination" id="5"/>
     <tableColumn name="Email Distribution List" id="6"/>
     <tableColumn name="Primary Contact Name" id="7"/>

</xml_diff>